<commit_message>
sycn rest transction files
</commit_message>
<xml_diff>
--- a/ChainSight 1st SIT/run_20250918_111143/module3/Module3Output_20250901.xlsx
+++ b/ChainSight 1st SIT/run_20250918_111143/module3/Module3Output_20250901.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang.s.37\OneDrive - Procter and Gamble\Documents\GitHub\chainsight\ChainSight 1st SIT\run_20250918_111143\module3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pgone-my.sharepoint.com/personal/zhang_s_37_pg_com/Documents/Documents/GitHub/chainsight/ChainSight 1st SIT/run_20250918_111143/module3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0944C424-DFEB-41C9-A77D-2FA6B16E17A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{0944C424-DFEB-41C9-A77D-2FA6B16E17A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2639D1D0-92A3-42FE-BB0B-6964F50480AB}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="4275" windowWidth="25185" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="792" yWindow="972" windowWidth="14760" windowHeight="10632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NetDemand" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>material</t>
   </si>
@@ -65,6 +78,18 @@
   </si>
   <si>
     <t>80813644</t>
+  </si>
+  <si>
+    <t>fcst</t>
+  </si>
+  <si>
+    <t>order/AO</t>
+  </si>
+  <si>
+    <t>inventory</t>
+  </si>
+  <si>
+    <t>in-transit</t>
   </si>
 </sst>
 </file>
@@ -72,7 +97,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -88,12 +113,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -123,12 +154,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,25 +464,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1048576"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +508,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -501,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -527,7 +560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -553,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -579,82 +612,122 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="4">
         <v>45902</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>-806</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="4">
         <v>45901</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="4">
         <v>45902</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>-435</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="4">
         <v>45901</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>45902</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>-806</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="4">
         <v>45901</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F10" s="3">
+        <f>F8-F7</f>
+        <v>-371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20">
+        <v>497</v>
+      </c>
+      <c r="G20" s="3">
+        <f>D20+E20-F20</f>
+        <v>-347</v>
       </c>
     </row>
   </sheetData>

</xml_diff>